<commit_message>
Our project was completed.
</commit_message>
<xml_diff>
--- a/src/test/java/resources/LoginData.xlsx
+++ b/src/test/java/resources/LoginData.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kuruçay Ailesi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kuruçay Ailesi\AppData\Local\Temp\Grup1_Internship_Project\src\test\java\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A986697E-670C-455A-927E-4FB6A73CBD77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B33C9F61-92AF-4D1A-A37A-CEC9E0ECD567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
+    <sheet name="Page1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>

</xml_diff>